<commit_message>
column-offset setting is supported
</commit_message>
<xml_diff>
--- a/example/demo.xlsx
+++ b/example/demo.xlsx
@@ -62,10 +62,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -525,7 +525,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -534,10 +534,10 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -546,7 +546,7 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1026,87 +1026,87 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A2:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="3" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="4" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
     <col min="2" max="2" width="26.1818181818182" customWidth="1"/>
     <col min="4" max="4" width="27.1818181818182" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="26" customHeight="1" spans="1:5">
-      <c r="A1" s="2" t="s">
+    <row r="2" ht="26" customHeight="1" spans="1:5">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2">
-        <v>222</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2">
-        <v>15866666002</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="B3" s="2"/>
       <c r="C3" s="2">
-        <v>23</v>
-      </c>
-      <c r="D3" s="2"/>
+        <v>222</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2">
+        <v>15866666002</v>
+      </c>
+      <c r="C4" s="2">
+        <v>23</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <v>15866666003</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C5" s="2">
         <v>31</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E5" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="15866666001@gmail.com"/>
-    <hyperlink ref="D4" r:id="rId2" display="15866666003@gmail.com" tooltip="mailto:15866666003@gmail.com"/>
+    <hyperlink ref="D3" r:id="rId1" display="15866666001@gmail.com"/>
+    <hyperlink ref="D5" r:id="rId2" display="15866666003@gmail.com" tooltip="mailto:15866666003@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>